<commit_message>
Improvement in playback sequence management
</commit_message>
<xml_diff>
--- a/wizardry/pin_defs.xlsx
+++ b/wizardry/pin_defs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\Projects\Ongoing\Progtomata\wizardry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206CBAEB-E3B7-4C17-930B-7B24A6D15D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E29A46C-8878-4C3D-B588-397901837595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,10 +530,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -826,7 +822,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Progress in audio playback management
</commit_message>
<xml_diff>
--- a/wizardry/pin_defs.xlsx
+++ b/wizardry/pin_defs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\Projects\Ongoing\Progtomata\wizardry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E29A46C-8878-4C3D-B588-397901837595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8CB5B4-DAFA-455F-8AFB-93554D8608A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="106">
   <si>
     <t>P1</t>
   </si>
@@ -332,13 +332,19 @@
   </si>
   <si>
     <t>BUTTON_1</t>
+  </si>
+  <si>
+    <t>OLED_SDA</t>
+  </si>
+  <si>
+    <t>OLED_SCL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +359,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC586C0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -491,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -514,6 +526,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -819,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,8 +845,8 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1030,11 +1045,15 @@
       <c r="F11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="H11" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1134,7 +1153,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1154,7 +1173,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>43</v>
       </c>
@@ -1176,7 +1195,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -1194,7 +1213,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
@@ -1214,7 +1233,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1236,7 +1255,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>27</v>
       </c>
@@ -1254,7 +1273,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
@@ -1276,7 +1295,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
@@ -1294,7 +1313,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
@@ -1312,7 +1331,7 @@
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
@@ -1329,6 +1348,12 @@
         <v>2</v>
       </c>
       <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N27" s="11"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>